<commit_message>
feat: update tabela motorola
</commit_message>
<xml_diff>
--- a/tabelas_template/DISPLAY MOTOROLA.xlsx
+++ b/tabelas_template/DISPLAY MOTOROLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tonilson\Downloads\pdf_fabiano\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712BC63B-EEAA-4BC3-B8B6-A156BA68ACC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D1447B-ABA7-40B6-A9DB-DCE147C44C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="210">
   <si>
     <t>DISPLAY MOTOROLA</t>
   </si>
@@ -720,9 +720,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 80,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -757,9 +754,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 50,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -794,9 +788,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 60,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -847,9 +838,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 75,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -874,9 +862,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 95,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -894,9 +879,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 65,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -939,9 +921,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 80,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -983,9 +962,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 105,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1027,9 +1003,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 60,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1064,9 +1037,6 @@
     </r>
   </si>
   <si>
-    <t>R$ 65,00</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1106,9 +1076,6 @@
       </rPr>
       <t xml:space="preserve"> (6 MESES DE GARANTIA)</t>
     </r>
-  </si>
-  <si>
-    <t>R$ 105,00</t>
   </si>
   <si>
     <r>
@@ -4213,7 +4180,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -4309,6 +4276,12 @@
     <font>
       <b/>
       <sz val="9.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -4433,7 +4406,7 @@
     <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4461,9 +4434,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4485,25 +4455,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4532,6 +4484,33 @@
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4817,8 +4796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4828,10 +4807,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4839,7 +4818,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="19">
         <v>50</v>
       </c>
     </row>
@@ -4847,7 +4826,7 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>120</v>
       </c>
     </row>
@@ -4855,7 +4834,7 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <v>120</v>
       </c>
     </row>
@@ -4863,7 +4842,7 @@
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="16">
         <v>175</v>
       </c>
     </row>
@@ -4871,7 +4850,7 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>45</v>
       </c>
     </row>
@@ -4879,7 +4858,7 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>55</v>
       </c>
     </row>
@@ -4887,7 +4866,7 @@
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>50</v>
       </c>
     </row>
@@ -4895,7 +4874,7 @@
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>50</v>
       </c>
     </row>
@@ -4903,7 +4882,7 @@
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>55</v>
       </c>
     </row>
@@ -4911,7 +4890,7 @@
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>60</v>
       </c>
     </row>
@@ -4919,7 +4898,7 @@
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>75</v>
       </c>
     </row>
@@ -4927,7 +4906,7 @@
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <v>85</v>
       </c>
     </row>
@@ -4935,7 +4914,7 @@
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <v>60</v>
       </c>
     </row>
@@ -4943,7 +4922,7 @@
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>75</v>
       </c>
     </row>
@@ -4951,7 +4930,7 @@
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="15">
         <v>85</v>
       </c>
     </row>
@@ -4959,7 +4938,7 @@
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="15">
         <v>50</v>
       </c>
     </row>
@@ -4967,7 +4946,7 @@
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="15">
         <v>60</v>
       </c>
     </row>
@@ -4975,7 +4954,7 @@
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="15">
         <v>85</v>
       </c>
     </row>
@@ -4983,7 +4962,7 @@
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="15">
         <v>50</v>
       </c>
     </row>
@@ -4991,7 +4970,7 @@
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="15">
         <v>60</v>
       </c>
     </row>
@@ -4999,231 +4978,231 @@
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>39</v>
+      <c r="B22" s="14">
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B23" s="14">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B24" s="14">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="B25" s="32">
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="B26" s="14">
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="B27" s="14">
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="B28" s="14">
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>58</v>
+        <v>50</v>
+      </c>
+      <c r="B29" s="14">
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="14">
         <v>60</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="B31" s="14">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A32" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>67</v>
+        <v>56</v>
+      </c>
+      <c r="B32" s="14">
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
-      <c r="A33" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="B33" s="10">
+      <c r="A33" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="B33" s="9">
         <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
-      <c r="A34" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="16">
+      <c r="A34" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="16">
+        <v>61</v>
+      </c>
+      <c r="B35" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.1" customHeight="1" thickBot="1">
       <c r="A36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="16">
+        <v>63</v>
+      </c>
+      <c r="B36" s="15">
         <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A37" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="16">
+        <v>65</v>
+      </c>
+      <c r="B37" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="16">
+        <v>67</v>
+      </c>
+      <c r="B38" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A39" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="16">
+        <v>69</v>
+      </c>
+      <c r="B39" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A40" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="16">
+        <v>71</v>
+      </c>
+      <c r="B40" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A41" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="16">
+        <v>73</v>
+      </c>
+      <c r="B41" s="15">
         <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A42" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="16">
+        <v>75</v>
+      </c>
+      <c r="B42" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A43" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="16">
+        <v>77</v>
+      </c>
+      <c r="B43" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A44" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="16">
+        <v>79</v>
+      </c>
+      <c r="B44" s="15">
         <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="16">
+        <v>81</v>
+      </c>
+      <c r="B45" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A46" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="16">
+        <v>83</v>
+      </c>
+      <c r="B46" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A47" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="16">
+        <v>85</v>
+      </c>
+      <c r="B47" s="15">
         <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A48" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="16">
+        <v>87</v>
+      </c>
+      <c r="B48" s="15">
         <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A49" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="16">
+        <v>88</v>
+      </c>
+      <c r="B49" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.95" customHeight="1" thickBot="1">
       <c r="A50" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="21">
+        <v>90</v>
+      </c>
+      <c r="B50" s="16">
         <v>50</v>
       </c>
     </row>
@@ -5231,7 +5210,7 @@
       <c r="A51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="16">
+      <c r="B51" s="15">
         <v>50</v>
       </c>
     </row>
@@ -5239,7 +5218,7 @@
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="16">
+      <c r="B52" s="15">
         <v>50</v>
       </c>
     </row>
@@ -5247,7 +5226,7 @@
       <c r="A53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="16">
+      <c r="B53" s="15">
         <v>50</v>
       </c>
     </row>
@@ -5255,7 +5234,7 @@
       <c r="A54" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="21">
+      <c r="B54" s="16">
         <v>70</v>
       </c>
     </row>
@@ -5263,7 +5242,7 @@
       <c r="A55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="16">
+      <c r="B55" s="15">
         <v>50</v>
       </c>
     </row>
@@ -5271,27 +5250,27 @@
       <c r="A56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="16">
+      <c r="B56" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="B57" s="22">
+      <c r="A57" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" s="28">
         <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A58" s="20"/>
-      <c r="B58" s="23"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="29"/>
     </row>
     <row r="59" spans="1:2" ht="15.75" thickBot="1">
       <c r="A59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="15">
         <v>55</v>
       </c>
     </row>
@@ -5299,7 +5278,7 @@
       <c r="A60" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B60" s="16">
+      <c r="B60" s="15">
         <v>45</v>
       </c>
     </row>
@@ -5307,27 +5286,27 @@
       <c r="A61" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B61" s="16">
+      <c r="B61" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="26.25" customHeight="1">
-      <c r="A62" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="B62" s="22">
+      <c r="A62" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="B62" s="28">
         <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A63" s="20"/>
-      <c r="B63" s="23"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="29"/>
     </row>
     <row r="64" spans="1:2" ht="15.75" thickBot="1">
       <c r="A64" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B64" s="16">
+      <c r="B64" s="15">
         <v>60</v>
       </c>
     </row>
@@ -5335,7 +5314,7 @@
       <c r="A65" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="16">
+      <c r="B65" s="15">
         <v>50</v>
       </c>
     </row>
@@ -5343,7 +5322,7 @@
       <c r="A66" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B66" s="16">
+      <c r="B66" s="15">
         <v>70</v>
       </c>
     </row>
@@ -5351,7 +5330,7 @@
       <c r="A67" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B67" s="16">
+      <c r="B67" s="15">
         <v>105</v>
       </c>
     </row>
@@ -5359,7 +5338,7 @@
       <c r="A68" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="16">
+      <c r="B68" s="15">
         <v>55</v>
       </c>
     </row>
@@ -5367,7 +5346,7 @@
       <c r="A69" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="14">
+      <c r="B69" s="13">
         <v>65</v>
       </c>
     </row>
@@ -5375,1164 +5354,1169 @@
       <c r="A70" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B70" s="16">
+      <c r="B70" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" thickBot="1">
       <c r="A71" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B71" s="16">
+        <v>39</v>
+      </c>
+      <c r="B71" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" thickBot="1">
       <c r="A72" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B72" s="16">
+        <v>41</v>
+      </c>
+      <c r="B72" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" thickBot="1">
       <c r="A73" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B73" s="16">
+        <v>43</v>
+      </c>
+      <c r="B73" s="15">
         <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="B74" s="22">
+      <c r="A74" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B74" s="28">
         <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A75" s="20"/>
-      <c r="B75" s="23"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="29"/>
     </row>
     <row r="76" spans="1:2" ht="15.75" thickBot="1">
       <c r="A76" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B76" s="16">
+        <v>47</v>
+      </c>
+      <c r="B76" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" thickBot="1">
       <c r="A77" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B77" s="16">
+        <v>49</v>
+      </c>
+      <c r="B77" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" thickBot="1">
       <c r="A78" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B78" s="16">
+        <v>51</v>
+      </c>
+      <c r="B78" s="15">
         <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" thickBot="1">
       <c r="A79" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B79" s="16">
+        <v>53</v>
+      </c>
+      <c r="B79" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" thickBot="1">
       <c r="A80" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B80" s="16">
+        <v>55</v>
+      </c>
+      <c r="B80" s="15">
         <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" thickBot="1">
       <c r="A81" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B81" s="16">
+        <v>57</v>
+      </c>
+      <c r="B81" s="15">
         <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" thickBot="1">
       <c r="A82" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B82" s="16">
+        <v>58</v>
+      </c>
+      <c r="B82" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" thickBot="1">
       <c r="A83" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B83" s="16">
+        <v>60</v>
+      </c>
+      <c r="B83" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.75" thickBot="1">
       <c r="A84" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B84" s="16">
+        <v>62</v>
+      </c>
+      <c r="B84" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" thickBot="1">
       <c r="A85" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B85" s="16">
+        <v>64</v>
+      </c>
+      <c r="B85" s="15">
         <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" thickBot="1">
       <c r="A86" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B86" s="16">
+        <v>66</v>
+      </c>
+      <c r="B86" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.75" thickBot="1">
       <c r="A87" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B87" s="16">
+        <v>68</v>
+      </c>
+      <c r="B87" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.75" thickBot="1">
       <c r="A88" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B88" s="16">
+        <v>70</v>
+      </c>
+      <c r="B88" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.75" thickBot="1">
       <c r="A89" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B89" s="16">
+        <v>72</v>
+      </c>
+      <c r="B89" s="15">
         <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.75" thickBot="1">
       <c r="A90" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B90" s="16">
+        <v>74</v>
+      </c>
+      <c r="B90" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" thickBot="1">
       <c r="A91" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B91" s="16">
+        <v>76</v>
+      </c>
+      <c r="B91" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.75" thickBot="1">
       <c r="A92" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B92" s="16">
+        <v>78</v>
+      </c>
+      <c r="B92" s="15">
         <v>115</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" thickBot="1">
       <c r="A93" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B93" s="16">
+        <v>80</v>
+      </c>
+      <c r="B93" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" thickBot="1">
       <c r="A94" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B94" s="16">
+        <v>82</v>
+      </c>
+      <c r="B94" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" thickBot="1">
       <c r="A95" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B95" s="16">
+        <v>84</v>
+      </c>
+      <c r="B95" s="15">
         <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.75" thickBot="1">
       <c r="A96" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B96" s="16">
+        <v>86</v>
+      </c>
+      <c r="B96" s="15">
         <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A97" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="B97" s="29">
+      <c r="A97" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B97" s="22">
         <v>60</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" thickBot="1">
       <c r="A98" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B98" s="28">
+        <v>89</v>
+      </c>
+      <c r="B98" s="21">
         <v>80</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.75" thickBot="1">
       <c r="A99" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B99" s="27">
+        <v>91</v>
+      </c>
+      <c r="B99" s="20">
         <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.75" thickBot="1">
       <c r="A100" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B100" s="30">
+        <v>92</v>
+      </c>
+      <c r="B100" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" thickBot="1">
       <c r="A101" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B101" s="26">
+        <v>93</v>
+      </c>
+      <c r="B101" s="19">
         <v>50</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.75" thickBot="1">
       <c r="A102" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B102" s="16">
+        <v>95</v>
+      </c>
+      <c r="B102" s="15">
         <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.75" thickBot="1">
       <c r="A103" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B103" s="16">
+        <v>97</v>
+      </c>
+      <c r="B103" s="15">
         <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.75" thickBot="1">
       <c r="A104" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B104" s="16">
+        <v>99</v>
+      </c>
+      <c r="B104" s="15">
         <v>175</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" thickBot="1">
       <c r="A105" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B105" s="16">
+        <v>101</v>
+      </c>
+      <c r="B105" s="15">
         <v>45</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.75" thickBot="1">
       <c r="A106" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B106" s="16">
+        <v>103</v>
+      </c>
+      <c r="B106" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.75" thickBot="1">
       <c r="A107" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B107" s="16">
+        <v>105</v>
+      </c>
+      <c r="B107" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.75" thickBot="1">
       <c r="A108" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B108" s="16">
+        <v>106</v>
+      </c>
+      <c r="B108" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.75" thickBot="1">
       <c r="A109" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B109" s="16">
+        <v>107</v>
+      </c>
+      <c r="B109" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.75" thickBot="1">
       <c r="A110" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B110" s="16">
+        <v>109</v>
+      </c>
+      <c r="B110" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.75" thickBot="1">
       <c r="A111" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B111" s="16">
+        <v>111</v>
+      </c>
+      <c r="B111" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.75" thickBot="1">
       <c r="A112" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B112" s="16">
+        <v>113</v>
+      </c>
+      <c r="B112" s="15">
         <v>85</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15.75" thickBot="1">
       <c r="A113" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B113" s="16">
+        <v>114</v>
+      </c>
+      <c r="B113" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15.75" thickBot="1">
       <c r="A114" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B114" s="16">
+        <v>115</v>
+      </c>
+      <c r="B114" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.75" thickBot="1">
       <c r="A115" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B115" s="16">
+        <v>117</v>
+      </c>
+      <c r="B115" s="15">
         <v>85</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.75" thickBot="1">
       <c r="A116" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B116" s="16">
+        <v>119</v>
+      </c>
+      <c r="B116" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.75" thickBot="1">
       <c r="A117" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B117" s="16">
+        <v>121</v>
+      </c>
+      <c r="B117" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A118" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B118" s="12">
+      <c r="A118" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B118" s="11">
         <v>85</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15.75" thickBot="1">
       <c r="A119" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B119" s="16">
+        <v>125</v>
+      </c>
+      <c r="B119" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15.75" thickBot="1">
       <c r="A120" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B120" s="16">
+        <v>127</v>
+      </c>
+      <c r="B120" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15.75" thickBot="1">
       <c r="A121" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B121" s="15">
+        <v>129</v>
+      </c>
+      <c r="B121" s="14">
         <v>60</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15.75" thickBot="1">
       <c r="A122" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B122" s="15">
+        <v>131</v>
+      </c>
+      <c r="B122" s="14">
         <v>70</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15.75" thickBot="1">
       <c r="A123" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B123" s="15">
+        <v>133</v>
+      </c>
+      <c r="B123" s="14">
         <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.75" thickBot="1">
       <c r="A124" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B124" s="15">
+        <v>135</v>
+      </c>
+      <c r="B124" s="14">
         <v>110</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15.75" thickBot="1">
       <c r="A125" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B125" s="15">
+        <v>136</v>
+      </c>
+      <c r="B125" s="14">
         <v>90</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15.75" thickBot="1">
       <c r="A126" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B126" s="15">
+        <v>137</v>
+      </c>
+      <c r="B126" s="14">
         <v>150</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15.75" thickBot="1">
       <c r="A127" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B127" s="15">
+        <v>139</v>
+      </c>
+      <c r="B127" s="14">
         <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15.75" thickBot="1">
       <c r="A128" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B128" s="15">
+        <v>141</v>
+      </c>
+      <c r="B128" s="14">
         <v>180</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15.75" thickBot="1">
       <c r="A129" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B129" s="15">
+        <v>143</v>
+      </c>
+      <c r="B129" s="14">
         <v>185</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.75" thickBot="1">
       <c r="A130" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B130" s="15">
+        <v>145</v>
+      </c>
+      <c r="B130" s="14">
         <v>195</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15.75" thickBot="1">
       <c r="A131" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B131" s="15">
+        <v>147</v>
+      </c>
+      <c r="B131" s="14">
         <v>190</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.75" thickBot="1">
       <c r="A132" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B132" s="31">
+        <v>202</v>
+      </c>
+      <c r="B132" s="24">
         <v>70</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15.75" thickBot="1">
       <c r="A133" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B133" s="16">
+        <v>150</v>
+      </c>
+      <c r="B133" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15.75" thickBot="1">
       <c r="A134" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B134" s="16">
+        <v>152</v>
+      </c>
+      <c r="B134" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15.75" thickBot="1">
       <c r="A135" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B135" s="16">
+        <v>154</v>
+      </c>
+      <c r="B135" s="15">
         <v>80</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15.75" thickBot="1">
       <c r="A136" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B136" s="16">
+        <v>156</v>
+      </c>
+      <c r="B136" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15.75" thickBot="1">
       <c r="A137" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B137" s="16">
+        <v>158</v>
+      </c>
+      <c r="B137" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15.75" thickBot="1">
       <c r="A138" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B138" s="16">
+        <v>160</v>
+      </c>
+      <c r="B138" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15.75" thickBot="1">
       <c r="A139" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B139" s="16">
+        <v>162</v>
+      </c>
+      <c r="B139" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15.75" thickBot="1">
       <c r="A140" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B140" s="16">
+        <v>164</v>
+      </c>
+      <c r="B140" s="15">
         <v>90</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.75" thickBot="1">
       <c r="A141" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B141" s="16">
+        <v>166</v>
+      </c>
+      <c r="B141" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15.75" thickBot="1">
       <c r="A142" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B142" s="16">
+        <v>168</v>
+      </c>
+      <c r="B142" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15.75" thickBot="1">
       <c r="A143" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B143" s="16">
+        <v>170</v>
+      </c>
+      <c r="B143" s="15">
         <v>95</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15.75" thickBot="1">
       <c r="A144" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B144" s="16">
+        <v>172</v>
+      </c>
+      <c r="B144" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.75" thickBot="1">
       <c r="A145" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B145" s="16">
+        <v>174</v>
+      </c>
+      <c r="B145" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15.75" thickBot="1">
       <c r="A146" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B146" s="16">
+        <v>176</v>
+      </c>
+      <c r="B146" s="15">
         <v>85</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15.75" thickBot="1">
       <c r="A147" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B147" s="16">
+        <v>178</v>
+      </c>
+      <c r="B147" s="15">
         <v>105</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.75" thickBot="1">
       <c r="A148" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B148" s="16">
+        <v>179</v>
+      </c>
+      <c r="B148" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.75" thickBot="1">
       <c r="A149" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B149" s="21">
+        <v>181</v>
+      </c>
+      <c r="B149" s="16">
         <v>50</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15.75" thickBot="1">
       <c r="A150" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B150" s="16">
+        <v>94</v>
+      </c>
+      <c r="B150" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15.75" thickBot="1">
       <c r="A151" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B151" s="16">
+        <v>96</v>
+      </c>
+      <c r="B151" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15.75" thickBot="1">
       <c r="A152" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B152" s="16">
+        <v>98</v>
+      </c>
+      <c r="B152" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15.75" thickBot="1">
       <c r="A153" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B153" s="16">
+        <v>100</v>
+      </c>
+      <c r="B153" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15.75" thickBot="1">
       <c r="A154" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B154" s="16">
+        <v>102</v>
+      </c>
+      <c r="B154" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15.75" thickBot="1">
       <c r="A155" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B155" s="16">
+        <v>104</v>
+      </c>
+      <c r="B155" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="156" spans="1:2">
-      <c r="A156" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="B156" s="22">
+      <c r="A156" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="B156" s="28">
         <v>85</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A157" s="20"/>
-      <c r="B157" s="23"/>
+      <c r="A157" s="27"/>
+      <c r="B157" s="29"/>
     </row>
     <row r="158" spans="1:2" ht="15.75" thickBot="1">
       <c r="A158" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B158" s="16">
+        <v>108</v>
+      </c>
+      <c r="B158" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15.75" thickBot="1">
       <c r="A159" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B159" s="16">
+        <v>110</v>
+      </c>
+      <c r="B159" s="15">
         <v>45</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15.75" thickBot="1">
       <c r="A160" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B160" s="16">
+        <v>112</v>
+      </c>
+      <c r="B160" s="15">
         <v>65</v>
       </c>
     </row>
     <row r="161" spans="1:2">
-      <c r="A161" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="B161" s="22">
+      <c r="A161" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="B161" s="28">
         <v>105</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A162" s="20"/>
-      <c r="B162" s="23"/>
+      <c r="A162" s="27"/>
+      <c r="B162" s="29"/>
     </row>
     <row r="163" spans="1:2" ht="15.75" thickBot="1">
       <c r="A163" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B163" s="16">
+        <v>116</v>
+      </c>
+      <c r="B163" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15.75" thickBot="1">
       <c r="A164" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B164" s="16">
+        <v>118</v>
+      </c>
+      <c r="B164" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15.75" thickBot="1">
       <c r="A165" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B165" s="16">
+        <v>120</v>
+      </c>
+      <c r="B165" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15.75" thickBot="1">
       <c r="A166" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B166" s="16">
+        <v>122</v>
+      </c>
+      <c r="B166" s="15">
         <v>105</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15.75" thickBot="1">
       <c r="A167" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B167" s="16">
+        <v>124</v>
+      </c>
+      <c r="B167" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15.75" thickBot="1">
       <c r="A168" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B168" s="14">
+        <v>126</v>
+      </c>
+      <c r="B168" s="13">
         <v>65</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15.75" thickBot="1">
       <c r="A169" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B169" s="16">
+        <v>128</v>
+      </c>
+      <c r="B169" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15.75" thickBot="1">
       <c r="A170" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B170" s="16">
+        <v>130</v>
+      </c>
+      <c r="B170" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15.75" thickBot="1">
       <c r="A171" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B171" s="16">
+        <v>132</v>
+      </c>
+      <c r="B171" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15.75" thickBot="1">
       <c r="A172" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B172" s="16">
+        <v>134</v>
+      </c>
+      <c r="B172" s="15">
         <v>90</v>
       </c>
     </row>
     <row r="173" spans="1:2">
-      <c r="A173" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="B173" s="22">
+      <c r="A173" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B173" s="28">
         <v>105</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A174" s="20"/>
-      <c r="B174" s="23"/>
+      <c r="A174" s="27"/>
+      <c r="B174" s="29"/>
     </row>
     <row r="175" spans="1:2" ht="15.75" thickBot="1">
       <c r="A175" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B175" s="16">
+        <v>138</v>
+      </c>
+      <c r="B175" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.75" thickBot="1">
       <c r="A176" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B176" s="16">
+        <v>140</v>
+      </c>
+      <c r="B176" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15.75" thickBot="1">
       <c r="A177" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B177" s="16">
+        <v>142</v>
+      </c>
+      <c r="B177" s="15">
         <v>130</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B178" s="16">
+        <v>144</v>
+      </c>
+      <c r="B178" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15.75" thickBot="1">
       <c r="A179" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B179" s="25">
+        <v>146</v>
+      </c>
+      <c r="B179" s="18">
         <v>95</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15.75" thickBot="1">
       <c r="A180" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B180" s="16">
+        <v>148</v>
+      </c>
+      <c r="B180" s="15">
         <v>130</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15.75" thickBot="1">
       <c r="A181" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B181" s="16">
+        <v>149</v>
+      </c>
+      <c r="B181" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="15.75" thickBot="1">
       <c r="A182" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B182" s="16">
+        <v>151</v>
+      </c>
+      <c r="B182" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="15.75" thickBot="1">
       <c r="A183" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B183" s="16">
+        <v>153</v>
+      </c>
+      <c r="B183" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15.75" thickBot="1">
       <c r="A184" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B184" s="16">
+        <v>155</v>
+      </c>
+      <c r="B184" s="15">
         <v>95</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="15.75" thickBot="1">
       <c r="A185" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B185" s="16">
+        <v>157</v>
+      </c>
+      <c r="B185" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B186" s="16">
+        <v>159</v>
+      </c>
+      <c r="B186" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15.75" thickBot="1">
       <c r="A187" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B187" s="25">
+        <v>161</v>
+      </c>
+      <c r="B187" s="18">
         <v>75</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15.75" thickBot="1">
       <c r="A188" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B188" s="16">
+        <v>163</v>
+      </c>
+      <c r="B188" s="15">
         <v>90</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15.75" thickBot="1">
       <c r="A189" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B189" s="16">
+        <v>165</v>
+      </c>
+      <c r="B189" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15.75" thickBot="1">
       <c r="A190" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B190" s="16">
+        <v>167</v>
+      </c>
+      <c r="B190" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="15.75" thickBot="1">
       <c r="A191" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B191" s="16">
+        <v>169</v>
+      </c>
+      <c r="B191" s="15">
         <v>115</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="15.75" thickBot="1">
       <c r="A192" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B192" s="16">
+        <v>171</v>
+      </c>
+      <c r="B192" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="15.75" thickBot="1">
       <c r="A193" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B193" s="16">
+        <v>173</v>
+      </c>
+      <c r="B193" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="15.75" thickBot="1">
       <c r="A194" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B194" s="16">
+        <v>175</v>
+      </c>
+      <c r="B194" s="15">
         <v>80</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15.75" thickBot="1">
       <c r="A195" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B195" s="16">
+        <v>177</v>
+      </c>
+      <c r="B195" s="15">
         <v>95</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A196" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="B196" s="29">
+      <c r="A196" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B196" s="22">
         <v>60</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="15.75" thickBot="1">
       <c r="A197" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B197" s="28">
+        <v>180</v>
+      </c>
+      <c r="B197" s="21">
         <v>80</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="15.75" thickBot="1">
       <c r="A198" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B198" s="27">
+        <v>182</v>
+      </c>
+      <c r="B198" s="20">
         <v>105</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15.75" thickBot="1">
       <c r="A199" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B199" s="32">
+        <v>183</v>
+      </c>
+      <c r="B199" s="25">
         <v>90</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15.75" thickBot="1">
       <c r="A200" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B200" s="26">
+        <v>184</v>
+      </c>
+      <c r="B200" s="19">
         <v>50</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="15.75" thickBot="1">
       <c r="A201" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B201" s="16">
+        <v>185</v>
+      </c>
+      <c r="B201" s="15">
         <v>120</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="15.75" thickBot="1">
       <c r="A202" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B202" s="16">
+        <v>186</v>
+      </c>
+      <c r="B202" s="15">
         <v>120</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="15.75" thickBot="1">
       <c r="A203" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B203" s="16">
+        <v>187</v>
+      </c>
+      <c r="B203" s="15">
         <v>175</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="30.75" thickBot="1">
       <c r="A204" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B204" s="24">
+        <v>188</v>
+      </c>
+      <c r="B204" s="17">
         <v>45</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="30.75" thickBot="1">
       <c r="A205" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B205" s="16">
+        <v>189</v>
+      </c>
+      <c r="B205" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="15.75" thickBot="1">
       <c r="A206" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B206" s="16">
+        <v>190</v>
+      </c>
+      <c r="B206" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="15.75" thickBot="1">
       <c r="A207" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B207" s="16">
+        <v>191</v>
+      </c>
+      <c r="B207" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="15.75" thickBot="1">
       <c r="A208" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B208" s="16">
+        <v>192</v>
+      </c>
+      <c r="B208" s="15">
         <v>55</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="15.75" thickBot="1">
       <c r="A209" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B209" s="16">
+        <v>193</v>
+      </c>
+      <c r="B209" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="15.75" thickBot="1">
       <c r="A210" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B210" s="16">
+        <v>194</v>
+      </c>
+      <c r="B210" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="15.75" thickBot="1">
       <c r="A211" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B211" s="16">
+        <v>195</v>
+      </c>
+      <c r="B211" s="15">
         <v>85</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="15.75" thickBot="1">
       <c r="A212" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B212" s="16">
+        <v>196</v>
+      </c>
+      <c r="B212" s="15">
         <v>60</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="15.75" thickBot="1">
       <c r="A213" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B213" s="16">
+        <v>197</v>
+      </c>
+      <c r="B213" s="15">
         <v>75</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="15.75" thickBot="1">
       <c r="A214" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B214" s="16">
+        <v>198</v>
+      </c>
+      <c r="B214" s="15">
         <v>85</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="30.75" thickBot="1">
       <c r="A215" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B215" s="16">
+        <v>199</v>
+      </c>
+      <c r="B215" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="15.75" thickBot="1">
       <c r="A216" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B216" s="21">
+        <v>200</v>
+      </c>
+      <c r="B216" s="16">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="B74:B75"/>
     <mergeCell ref="A173:A174"/>
@@ -6541,11 +6525,6 @@
     <mergeCell ref="B156:B157"/>
     <mergeCell ref="A161:A162"/>
     <mergeCell ref="B161:B162"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>